<commit_message>
update testcases personal loan apply page 20230215
</commit_message>
<xml_diff>
--- a/test_data/test_scenario_krungsri.xlsx
+++ b/test_data/test_scenario_krungsri.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kittipong.t\Desktop\practice\practice-robotframework\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kittipong.t\Desktop\practice\RobotFrameworkPractice\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C527DA4-BF46-4477-BF24-70C6A6C28B80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680AD278-7A62-4B86-8ECB-992F8F3D3BC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="2" xr2:uid="{4ED66F88-68C3-4300-AFE7-6B8843B977A8}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="74">
   <si>
     <t>name</t>
   </si>
@@ -331,7 +331,7 @@
     <t>กรุณากรอกชื่อ</t>
   </si>
   <si>
-    <t>""</t>
+    <t>0600000000</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -484,6 +484,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -888,113 +889,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="18" t="s">
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1019,7 +1020,7 @@
       <c r="L7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="19"/>
+      <c r="M7" s="20"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
@@ -1028,7 +1029,7 @@
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="21" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1066,7 +1067,7 @@
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1102,7 +1103,7 @@
       <c r="B10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="21"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="1" t="s">
         <v>44</v>
       </c>
@@ -1138,7 +1139,7 @@
       <c r="B11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="1" t="s">
         <v>45</v>
       </c>
@@ -1174,7 +1175,7 @@
       <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1210,7 +1211,7 @@
       <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1246,7 +1247,7 @@
       <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="21"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1282,7 +1283,7 @@
       <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1318,7 +1319,7 @@
       <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="21"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1354,7 +1355,7 @@
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1390,7 +1391,7 @@
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="21"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1461,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915139F8-51A1-4A8B-A65C-E1A4E7A63C58}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,9 +1510,7 @@
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1521,7 +1520,7 @@
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1541,16 +1540,14 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -1573,13 +1570,11 @@
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -1605,10 +1600,8 @@
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -1637,7 +1630,7 @@
       <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -1664,9 +1657,9 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -1695,7 +1688,7 @@
       <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -1724,7 +1717,7 @@
       <c r="E9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -1753,15 +1746,13 @@
       <c r="E10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="H10" s="3"/>
       <c r="I10" s="3" t="s">
         <v>16</v>
       </c>
@@ -1782,7 +1773,7 @@
       <c r="E11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -1791,9 +1782,7 @@
       <c r="H11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1811,7 +1800,7 @@
       <c r="E12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -1827,6 +1816,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2:E4 E6:E12 D2:D3 D5:D12" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1853,12 +1845,12 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1890,9 +1882,7 @@
       <c r="A4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="B4" s="9"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -1913,11 +1903,10 @@
       <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>54</v>
-      </c>
+      <c r="A8" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>